<commit_message>
cleaning files + new points
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leocr\Desktop\bot-autohotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8743CAFE-F5BD-4FC6-BBBC-D6A8B3394E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D99F246-8CA0-47FC-84CD-F16F3CF49D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="bot" sheetId="1" r:id="rId1"/>
-    <sheet name="9" sheetId="2" r:id="rId2"/>
+    <sheet name="9" sheetId="2" r:id="rId1"/>
+    <sheet name="bot" sheetId="1" r:id="rId2"/>
     <sheet name="8" sheetId="3" r:id="rId3"/>
     <sheet name="7" sheetId="4" r:id="rId4"/>
     <sheet name="6" sheetId="5" r:id="rId5"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="329">
   <si>
     <t>title</t>
   </si>
@@ -1580,6 +1580,9 @@
   </si>
   <si>
     <t>Déménagement00010</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -1882,11 +1885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1947,19 +1950,19 @@
     </row>
     <row r="2" spans="1:16" ht="33.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>59</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1" t="str">
         <f>"0156374553"</f>
@@ -1969,150 +1972,162 @@
         <f>"0171183931"</f>
         <v>0171183931</v>
       </c>
+      <c r="I2" s="2" t="str">
+        <f>"0187660267"</f>
+        <v>0187660267</v>
+      </c>
+      <c r="J2" s="1" t="str">
+        <f>"0184807351"</f>
+        <v>0184807351</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>"0187660694"</f>
+        <v>0187660694</v>
+      </c>
     </row>
     <row r="3" spans="1:16" ht="24.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="29.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
+      <c r="A5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
       </c>
       <c r="G5" s="2">
         <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="31.5" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
+      <c r="A6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="27" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>36</v>
+      <c r="A7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2</v>
+        <v>81</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>41</v>
+      <c r="A8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="25.5" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>46</v>
+      <c r="A9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2</v>
+        <v>89</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>50</v>
+      <c r="A10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>93</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -2122,17 +2137,17 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.5" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>55</v>
+      <c r="A11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>97</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -2141,34 +2156,163 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:16" ht="15" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1">
+      <c r="A15" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15" customHeight="1">
+      <c r="A17" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" customHeight="1">
+      <c r="A19" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A21" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A25" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A28" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A29" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A30" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A31" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A32" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A33" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A34" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A35" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A36" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A37" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A38" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A39" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A40" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A41" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:1" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -4384,10 +4528,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -4447,19 +4593,19 @@
     </row>
     <row r="2" spans="1:16" ht="33.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>60</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1" t="str">
         <f>"0156374553"</f>
@@ -4469,162 +4615,150 @@
         <f>"0171183931"</f>
         <v>0171183931</v>
       </c>
-      <c r="I2" s="2" t="str">
-        <f>"0187660267"</f>
-        <v>0187660267</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f>"0184807351"</f>
-        <v>0184807351</v>
-      </c>
-      <c r="K2" s="1" t="str">
-        <f>"0187660694"</f>
-        <v>0187660694</v>
-      </c>
     </row>
     <row r="3" spans="1:16" ht="24.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>64</v>
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>68</v>
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="29.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>72</v>
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
       </c>
       <c r="G5" s="2">
         <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="31.5" customHeight="1">
-      <c r="A6" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>76</v>
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2</v>
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="27" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>80</v>
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3</v>
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>84</v>
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="2">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="25.5" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>88</v>
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>92</v>
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>94</v>
+        <v>51</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -4634,17 +4768,17 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.5" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>96</v>
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>98</v>
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
bot working on the new windows 15 inches screen
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leocr\Desktop\bot-autohotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D99F246-8CA0-47FC-84CD-F16F3CF49D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2D16E0-CA5A-49E5-A787-54106373C016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="0" windowWidth="23280" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="2" r:id="rId1"/>
@@ -1888,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1962,11 +1962,10 @@
         <v>62</v>
       </c>
       <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <f>"0156374553"</f>
-        <v>0156374553</v>
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>156374553</v>
       </c>
       <c r="H2" s="1" t="str">
         <f>"0171183931"</f>

</xml_diff>